<commit_message>
Minor revision on ``IEEET3`` example file.
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_ieeet3.xlsx
+++ b/andes/cases/ieee14/ieee14_ieeet3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/andes/andes/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06741E85-13A1-9546-A3B9-89F89789740B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1062572-C49A-B74D-A732-DCA27DE002F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1896,7 +1896,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>